<commit_message>
Added a comparison between the DBs
</commit_message>
<xml_diff>
--- a/python/Statistics/Results/RST_classification_NCEP_1979-2016.xlsx
+++ b/python/Statistics/Results/RST_classification_NCEP_1979-2016.xlsx
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="X2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2" t="s">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" t="s">
         <v>0</v>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="s">
         <v>0</v>
@@ -554,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="X3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y3" t="s">
         <v>0</v>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="U4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V4" t="s">
         <v>2</v>
@@ -685,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="AC4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD4" t="s">
         <v>3</v>
@@ -709,7 +709,7 @@
         <v>1</v>
       </c>
       <c r="AK4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL4" t="s">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="P6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="s">
         <v>0</v>
@@ -970,7 +970,7 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" t="s">
         <v>0</v>
@@ -979,7 +979,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="s">
         <v>0</v>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="AC7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7" t="s">
         <v>0</v>
@@ -1235,13 +1235,13 @@
         <v>0</v>
       </c>
       <c r="S9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T9" t="s">
         <v>0</v>
       </c>
       <c r="U9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V9" t="s">
         <v>0</v>
@@ -1303,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
         <v>0</v>
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="U10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V10" t="s">
         <v>0</v>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="Q11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R11" t="s">
         <v>0</v>
@@ -1485,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z11" t="s">
         <v>1</v>
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="AD11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AE11" t="s">
         <v>1</v>
@@ -1595,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="W12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12" t="s">
         <v>1</v>
@@ -1625,7 +1625,7 @@
         <v>0</v>
       </c>
       <c r="AG12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH12" t="s">
         <v>0</v>
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="AL12" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM12" t="s">
         <v>1</v>
@@ -1714,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="X13" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" t="s">
         <v>1</v>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" t="s">
         <v>0</v>
@@ -1925,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="Q15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15" t="s">
         <v>1</v>
@@ -1934,7 +1934,7 @@
         <v>1</v>
       </c>
       <c r="T15" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U15" t="s">
         <v>0</v>
@@ -1961,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="AC15" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD15" t="s">
         <v>1</v>
@@ -2011,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="s">
         <v>0</v>
@@ -2032,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" t="s">
         <v>0</v>
@@ -2136,7 +2136,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" t="s">
         <v>0</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q17" t="s">
         <v>0</v>
@@ -2172,7 +2172,7 @@
         <v>0</v>
       </c>
       <c r="V17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W17" t="s">
         <v>1</v>
@@ -2199,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="AE17" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF17" t="s">
         <v>2</v>
@@ -2315,13 +2315,13 @@
         <v>1</v>
       </c>
       <c r="AE18" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF18" t="s">
         <v>0</v>
       </c>
       <c r="AG18" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH18" t="s">
         <v>1</v>
@@ -2535,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="AA20" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB20" t="s">
         <v>0</v>
@@ -2788,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="AH22" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI22" t="s">
         <v>0</v>
@@ -2811,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>0</v>
@@ -2895,7 +2895,7 @@
         <v>0</v>
       </c>
       <c r="AE23" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF23" t="s">
         <v>0</v>
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="T24" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U24" t="s">
         <v>0</v>
@@ -3264,7 +3264,7 @@
         <v>0</v>
       </c>
       <c r="AL26" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM26" t="s">
         <v>0</v>
@@ -3341,7 +3341,7 @@
         <v>0</v>
       </c>
       <c r="Y27" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z27" t="s">
         <v>0</v>
@@ -3359,7 +3359,7 @@
         <v>1</v>
       </c>
       <c r="AE27" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF27" t="s">
         <v>0</v>
@@ -3397,7 +3397,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
         <v>1</v>
@@ -3552,7 +3552,7 @@
         <v>0</v>
       </c>
       <c r="R29" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S29" t="s">
         <v>0</v>
@@ -3695,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="AA30" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB30" t="s">
         <v>0</v>
@@ -3873,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
         <v>2</v>
@@ -3909,13 +3909,13 @@
         <v>0</v>
       </c>
       <c r="U32" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V32" t="s">
         <v>1</v>
       </c>
       <c r="W32" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X32" t="s">
         <v>0</v>
@@ -3936,7 +3936,7 @@
         <v>1</v>
       </c>
       <c r="AD32" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AE32" t="s">
         <v>0</v>
@@ -3998,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="L33" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" t="s">
         <v>1</v>
@@ -4123,7 +4123,7 @@
         <v>0</v>
       </c>
       <c r="O34" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P34" t="s">
         <v>0</v>
@@ -4144,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="V34" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W34" t="s">
         <v>0</v>
@@ -4209,7 +4209,7 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F35" t="s">
         <v>0</v>
@@ -4296,10 +4296,10 @@
         <v>0</v>
       </c>
       <c r="AH35" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI35" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ35" t="s">
         <v>0</v>
@@ -4343,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="K36" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L36" t="s">
         <v>1</v>
@@ -4391,7 +4391,7 @@
         <v>0</v>
       </c>
       <c r="AA36" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB36" t="s">
         <v>0</v>
@@ -4406,7 +4406,7 @@
         <v>2</v>
       </c>
       <c r="AF36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG36" t="s">
         <v>0</v>
@@ -4447,7 +4447,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H37" t="s">
         <v>0</v>
@@ -4507,13 +4507,13 @@
         <v>0</v>
       </c>
       <c r="AA37" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB37" t="s">
         <v>0</v>
       </c>
       <c r="AC37" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD37" t="s">
         <v>0</v>
@@ -5007,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="AM41" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:39">
@@ -5018,7 +5018,7 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
@@ -5054,7 +5054,7 @@
         <v>0</v>
       </c>
       <c r="P42" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q42" t="s">
         <v>0</v>
@@ -5066,10 +5066,10 @@
         <v>0</v>
       </c>
       <c r="T42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V42" t="s">
         <v>1</v>
@@ -5286,7 +5286,7 @@
         <v>0</v>
       </c>
       <c r="P44" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q44" t="s">
         <v>0</v>
@@ -5343,7 +5343,7 @@
         <v>0</v>
       </c>
       <c r="AI44" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ44" t="s">
         <v>0</v>
@@ -5402,7 +5402,7 @@
         <v>0</v>
       </c>
       <c r="P45" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q45" t="s">
         <v>0</v>
@@ -5670,7 +5670,7 @@
         <v>0</v>
       </c>
       <c r="AB47" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC47" t="s">
         <v>0</v>
@@ -5765,7 +5765,7 @@
         <v>1</v>
       </c>
       <c r="U48" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V48" t="s">
         <v>0</v>
@@ -5819,7 +5819,7 @@
         <v>0</v>
       </c>
       <c r="AM48" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:39">
@@ -5845,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="s">
         <v>0</v>
@@ -6098,7 +6098,7 @@
         <v>0</v>
       </c>
       <c r="P51" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q51" t="s">
         <v>2</v>
@@ -6113,7 +6113,7 @@
         <v>0</v>
       </c>
       <c r="U51" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V51" t="s">
         <v>0</v>
@@ -6291,7 +6291,7 @@
         <v>0</v>
       </c>
       <c r="C53" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="s">
         <v>0</v>
@@ -6387,7 +6387,7 @@
         <v>0</v>
       </c>
       <c r="AI53" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ53" t="s">
         <v>0</v>
@@ -6541,7 +6541,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" t="s">
         <v>0</v>
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
       <c r="M55" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N55" t="s">
         <v>1</v>
@@ -6583,7 +6583,7 @@
         <v>1</v>
       </c>
       <c r="W55" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X55" t="s">
         <v>0</v>
@@ -6601,13 +6601,13 @@
         <v>1</v>
       </c>
       <c r="AC55" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD55" t="s">
         <v>2</v>
       </c>
       <c r="AE55" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF55" t="s">
         <v>0</v>
@@ -6639,7 +6639,7 @@
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
         <v>0</v>
@@ -6672,7 +6672,7 @@
         <v>0</v>
       </c>
       <c r="N56" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O56" t="s">
         <v>0</v>
@@ -6863,7 +6863,7 @@
         <v>0</v>
       </c>
       <c r="AM57" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:39">
@@ -6928,7 +6928,7 @@
         <v>0</v>
       </c>
       <c r="V58" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W58" t="s">
         <v>1</v>
@@ -6987,7 +6987,7 @@
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
@@ -7005,7 +7005,7 @@
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59" t="s">
         <v>0</v>
@@ -7044,7 +7044,7 @@
         <v>1</v>
       </c>
       <c r="V59" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W59" t="s">
         <v>0</v>
@@ -7160,7 +7160,7 @@
         <v>0</v>
       </c>
       <c r="V60" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W60" t="s">
         <v>3</v>
@@ -7181,13 +7181,13 @@
         <v>0</v>
       </c>
       <c r="AC60" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD60" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE60" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF60" t="s">
         <v>0</v>
@@ -7323,7 +7323,7 @@
         <v>0</v>
       </c>
       <c r="AA62" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB62" t="s">
         <v>0</v>
@@ -7510,7 +7510,7 @@
         <v>0</v>
       </c>
       <c r="L64" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M64" t="s">
         <v>0</v>
@@ -7632,7 +7632,7 @@
         <v>0</v>
       </c>
       <c r="N65" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O65" t="s">
         <v>0</v>
@@ -7718,7 +7718,7 @@
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
         <v>1</v>
@@ -8004,7 +8004,7 @@
         <v>0</v>
       </c>
       <c r="V68" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W68" t="s">
         <v>0</v>
@@ -8043,7 +8043,7 @@
         <v>0</v>
       </c>
       <c r="AI68" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ68" t="s">
         <v>0</v>
@@ -8126,7 +8126,7 @@
         <v>0</v>
       </c>
       <c r="X69" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y69" t="s">
         <v>0</v>
@@ -8165,7 +8165,7 @@
         <v>2</v>
       </c>
       <c r="AK69" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL69" t="s">
         <v>1</v>
@@ -8263,7 +8263,7 @@
         <v>0</v>
       </c>
       <c r="AE70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF70" t="s">
         <v>0</v>
@@ -8284,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="AL70" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM70" t="s">
         <v>2</v>
@@ -8298,7 +8298,7 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E71" t="s">
         <v>0</v>
@@ -8462,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="T72" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U72" t="s">
         <v>0</v>
@@ -8733,7 +8733,7 @@
         <v>0</v>
       </c>
       <c r="AG74" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH74" t="s">
         <v>0</v>
@@ -8864,7 +8864,7 @@
         <v>0</v>
       </c>
       <c r="AL75" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM75" t="s">
         <v>0</v>
@@ -9024,10 +9024,10 @@
         <v>1</v>
       </c>
       <c r="N77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O77" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P77" t="s">
         <v>1</v>
@@ -9051,13 +9051,13 @@
         <v>1</v>
       </c>
       <c r="W77" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X77" t="s">
         <v>0</v>
       </c>
       <c r="Y77" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z77" t="s">
         <v>0</v>
@@ -9137,7 +9137,7 @@
         <v>0</v>
       </c>
       <c r="M78" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N78" t="s">
         <v>2</v>
@@ -9146,7 +9146,7 @@
         <v>0</v>
       </c>
       <c r="P78" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q78" t="s">
         <v>1</v>
@@ -9455,7 +9455,7 @@
         <v>0</v>
       </c>
       <c r="C81" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D81" t="s">
         <v>0</v>
@@ -9485,7 +9485,7 @@
         <v>0</v>
       </c>
       <c r="M81" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N81" t="s">
         <v>1</v>
@@ -9601,7 +9601,7 @@
         <v>0</v>
       </c>
       <c r="M82" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N82" t="s">
         <v>0</v>
@@ -9616,7 +9616,7 @@
         <v>0</v>
       </c>
       <c r="R82" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S82" t="s">
         <v>0</v>
@@ -9661,13 +9661,13 @@
         <v>0</v>
       </c>
       <c r="AG82" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH82" t="s">
         <v>0</v>
       </c>
       <c r="AI82" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ82" t="s">
         <v>0</v>
@@ -9777,7 +9777,7 @@
         <v>0</v>
       </c>
       <c r="AG83" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH83" t="s">
         <v>0</v>
@@ -9890,10 +9890,10 @@
         <v>0</v>
       </c>
       <c r="AF84" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG84" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH84" t="s">
         <v>0</v>
@@ -9919,7 +9919,7 @@
         <v>0</v>
       </c>
       <c r="C85" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D85" t="s">
         <v>0</v>
@@ -10038,7 +10038,7 @@
         <v>0</v>
       </c>
       <c r="D86" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86" t="s">
         <v>3</v>
@@ -10131,7 +10131,7 @@
         <v>0</v>
       </c>
       <c r="AI86" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ86" t="s">
         <v>1</v>
@@ -10282,10 +10282,10 @@
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I88" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J88" t="s">
         <v>0</v>
@@ -10339,7 +10339,7 @@
         <v>0</v>
       </c>
       <c r="AA88" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB88" t="s">
         <v>1</v>
@@ -10401,7 +10401,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J89" t="s">
         <v>1</v>
@@ -10446,7 +10446,7 @@
         <v>1</v>
       </c>
       <c r="X89" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y89" t="s">
         <v>0</v>
@@ -10556,7 +10556,7 @@
         <v>0</v>
       </c>
       <c r="V90" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W90" t="s">
         <v>1</v>
@@ -10568,7 +10568,7 @@
         <v>0</v>
       </c>
       <c r="Z90" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA90" t="s">
         <v>1</v>
@@ -10734,7 +10734,7 @@
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E92" t="s">
         <v>1</v>
@@ -10865,10 +10865,10 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J93" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K93" t="s">
         <v>1</v>
@@ -11076,7 +11076,7 @@
     </row>
     <row r="95" spans="1:39">
       <c r="B95" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C95" t="s">
         <v>0</v>
@@ -11151,7 +11151,7 @@
         <v>2</v>
       </c>
       <c r="AA95" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB95" t="s">
         <v>0</v>
@@ -11368,7 +11368,7 @@
         <v>0</v>
       </c>
       <c r="V97" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W97" t="s">
         <v>0</v>
@@ -11401,13 +11401,13 @@
         <v>0</v>
       </c>
       <c r="AG97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH97" t="s">
         <v>0</v>
       </c>
       <c r="AI97" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ97" t="s">
         <v>0</v>
@@ -11433,7 +11433,7 @@
         <v>0</v>
       </c>
       <c r="E98" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" t="s">
         <v>0</v>
@@ -11472,7 +11472,7 @@
         <v>0</v>
       </c>
       <c r="R98" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S98" t="s">
         <v>0</v>
@@ -11487,7 +11487,7 @@
         <v>0</v>
       </c>
       <c r="W98" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X98" t="s">
         <v>0</v>
@@ -11606,7 +11606,7 @@
         <v>0</v>
       </c>
       <c r="X99" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y99" t="s">
         <v>0</v>
@@ -11737,7 +11737,7 @@
         <v>1</v>
       </c>
       <c r="AC100" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD100" t="s">
         <v>0</v>
@@ -11781,7 +11781,7 @@
         <v>0</v>
       </c>
       <c r="E101" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F101" t="s">
         <v>0</v>
@@ -11945,7 +11945,7 @@
         <v>0</v>
       </c>
       <c r="U102" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V102" t="s">
         <v>0</v>
@@ -11975,7 +11975,7 @@
         <v>0</v>
       </c>
       <c r="AE102" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF102" t="s">
         <v>0</v>
@@ -12281,7 +12281,7 @@
         <v>0</v>
       </c>
       <c r="Q105" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R105" t="s">
         <v>2</v>
@@ -12397,7 +12397,7 @@
         <v>0</v>
       </c>
       <c r="Q106" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R106" t="s">
         <v>0</v>
@@ -12409,7 +12409,7 @@
         <v>0</v>
       </c>
       <c r="U106" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V106" t="s">
         <v>0</v>
@@ -12439,7 +12439,7 @@
         <v>0</v>
       </c>
       <c r="AE106" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF106" t="s">
         <v>2</v>
@@ -12540,7 +12540,7 @@
         <v>2</v>
       </c>
       <c r="Z107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA107" t="s">
         <v>0</v>
@@ -12653,7 +12653,7 @@
         <v>0</v>
       </c>
       <c r="Y108" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z108" t="s">
         <v>0</v>
@@ -12689,7 +12689,7 @@
         <v>0</v>
       </c>
       <c r="AK108" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL108" t="s">
         <v>0</v>
@@ -12757,7 +12757,7 @@
         <v>0</v>
       </c>
       <c r="U109" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V109" t="s">
         <v>0</v>
@@ -12962,10 +12962,10 @@
         <v>0</v>
       </c>
       <c r="L111" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M111" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N111" t="s">
         <v>0</v>
@@ -13054,7 +13054,7 @@
         <v>0</v>
       </c>
       <c r="D112" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" t="s">
         <v>0</v>
@@ -13159,7 +13159,7 @@
         <v>0</v>
       </c>
       <c r="AM112" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:39">
@@ -13438,7 +13438,7 @@
         <v>1</v>
       </c>
       <c r="P115" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q115" t="s">
         <v>0</v>
@@ -13846,7 +13846,7 @@
         <v>0</v>
       </c>
       <c r="AJ118" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK118" t="s">
         <v>0</v>
@@ -13908,7 +13908,7 @@
         <v>0</v>
       </c>
       <c r="R119" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S119" t="s">
         <v>1</v>
@@ -13950,7 +13950,7 @@
         <v>0</v>
       </c>
       <c r="AF119" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG119" t="s">
         <v>0</v>
@@ -13962,13 +13962,13 @@
         <v>0</v>
       </c>
       <c r="AJ119" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK119" t="s">
         <v>0</v>
       </c>
       <c r="AL119" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM119" t="s">
         <v>0</v>
@@ -14131,7 +14131,7 @@
         <v>0</v>
       </c>
       <c r="O121" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P121" t="s">
         <v>1</v>
@@ -14158,7 +14158,7 @@
         <v>0</v>
       </c>
       <c r="X121" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y121" t="s">
         <v>0</v>
@@ -14280,7 +14280,7 @@
         <v>0</v>
       </c>
       <c r="Z122" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA122" t="s">
         <v>0</v>
@@ -14423,7 +14423,7 @@
         <v>0</v>
       </c>
       <c r="AI123" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ123" t="s">
         <v>0</v>
@@ -14586,7 +14586,7 @@
         <v>1</v>
       </c>
       <c r="L125" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M125" t="s">
         <v>0</v>
@@ -14699,7 +14699,7 @@
         <v>0</v>
       </c>
       <c r="K126" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L126" t="s">
         <v>1</v>
@@ -14744,7 +14744,7 @@
         <v>0</v>
       </c>
       <c r="Z126" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA126" t="s">
         <v>0</v>
@@ -14768,7 +14768,7 @@
         <v>0</v>
       </c>
       <c r="AH126" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI126" t="s">
         <v>0</v>
@@ -15020,7 +15020,7 @@
     </row>
     <row r="129" spans="1:39">
       <c r="B129" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C129" t="s">
         <v>1</v>
@@ -15041,7 +15041,7 @@
         <v>0</v>
       </c>
       <c r="I129" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J129" t="s">
         <v>2</v>
@@ -15077,7 +15077,7 @@
         <v>0</v>
       </c>
       <c r="U129" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V129" t="s">
         <v>0</v>
@@ -15104,7 +15104,7 @@
         <v>0</v>
       </c>
       <c r="AD129" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE129" t="s">
         <v>0</v>
@@ -15172,7 +15172,7 @@
         <v>0</v>
       </c>
       <c r="N130" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O130" t="s">
         <v>0</v>
@@ -15309,7 +15309,7 @@
         <v>0</v>
       </c>
       <c r="U131" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V131" t="s">
         <v>0</v>
@@ -15672,7 +15672,7 @@
         <v>0</v>
       </c>
       <c r="Z134" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA134" t="s">
         <v>0</v>
@@ -15728,7 +15728,7 @@
         <v>0</v>
       </c>
       <c r="F135" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G135" t="s">
         <v>1</v>
@@ -15746,7 +15746,7 @@
         <v>0</v>
       </c>
       <c r="L135" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M135" t="s">
         <v>0</v>
@@ -15978,7 +15978,7 @@
         <v>2</v>
       </c>
       <c r="L137" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M137" t="s">
         <v>1</v>
@@ -16374,7 +16374,7 @@
         <v>0</v>
       </c>
       <c r="AB140" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC140" t="s">
         <v>0</v>
@@ -16683,7 +16683,7 @@
         <v>0</v>
       </c>
       <c r="O143" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P143" t="s">
         <v>0</v>
@@ -16749,7 +16749,7 @@
         <v>0</v>
       </c>
       <c r="AK143" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL143" t="s">
         <v>0</v>
@@ -16790,7 +16790,7 @@
         <v>0</v>
       </c>
       <c r="L144" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M144" t="s">
         <v>0</v>
@@ -16820,7 +16820,7 @@
         <v>0</v>
       </c>
       <c r="V144" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W144" t="s">
         <v>0</v>
@@ -16936,7 +16936,7 @@
         <v>0</v>
       </c>
       <c r="V145" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W145" t="s">
         <v>0</v>
@@ -16998,7 +16998,7 @@
         <v>1</v>
       </c>
       <c r="D146" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E146" t="s">
         <v>0</v>
@@ -17007,7 +17007,7 @@
         <v>0</v>
       </c>
       <c r="G146" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H146" t="s">
         <v>0</v>
@@ -17049,7 +17049,7 @@
         <v>0</v>
       </c>
       <c r="U146" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V146" t="s">
         <v>1</v>
@@ -17058,7 +17058,7 @@
         <v>0</v>
       </c>
       <c r="X146" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y146" t="s">
         <v>0</v>
@@ -17114,7 +17114,7 @@
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E147" t="s">
         <v>0</v>
@@ -17486,7 +17486,7 @@
         <v>0</v>
       </c>
       <c r="L150" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M150" t="s">
         <v>1</v>
@@ -17516,7 +17516,7 @@
         <v>0</v>
       </c>
       <c r="V150" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W150" t="s">
         <v>0</v>
@@ -17691,7 +17691,7 @@
         <v>0</v>
       </c>
       <c r="C152" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D152" t="s">
         <v>1</v>
@@ -17941,7 +17941,7 @@
         <v>0</v>
       </c>
       <c r="I154" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J154" t="s">
         <v>0</v>
@@ -18036,7 +18036,7 @@
     </row>
     <row r="155" spans="1:39">
       <c r="B155" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C155" t="s">
         <v>0</v>
@@ -18170,7 +18170,7 @@
         <v>0</v>
       </c>
       <c r="H156" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I156" t="s">
         <v>0</v>
@@ -18456,10 +18456,10 @@
         <v>0</v>
       </c>
       <c r="Z158" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA158" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB158" t="s">
         <v>0</v>
@@ -18524,7 +18524,7 @@
         <v>0</v>
       </c>
       <c r="J159" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K159" t="s">
         <v>1</v>
@@ -18935,7 +18935,7 @@
         <v>0</v>
       </c>
       <c r="AE162" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF162" t="s">
         <v>0</v>
@@ -19063,7 +19063,7 @@
         <v>0</v>
       </c>
       <c r="AI163" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ163" t="s">
         <v>0</v>
@@ -19173,7 +19173,7 @@
         <v>0</v>
       </c>
       <c r="AG164" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH164" t="s">
         <v>0</v>
@@ -20133,7 +20133,7 @@
         <v>0</v>
       </c>
       <c r="E173" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F173" t="s">
         <v>0</v>
@@ -20303,7 +20303,7 @@
         <v>0</v>
       </c>
       <c r="W174" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X174" t="s">
         <v>0</v>
@@ -20389,7 +20389,7 @@
         <v>0</v>
       </c>
       <c r="M175" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N175" t="s">
         <v>0</v>
@@ -22891,7 +22891,7 @@
         <v>0</v>
       </c>
       <c r="AI196" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ196" t="s">
         <v>0</v>
@@ -23679,7 +23679,7 @@
         <v>0</v>
       </c>
       <c r="AA203" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB203" t="s">
         <v>0</v>
@@ -24875,7 +24875,7 @@
         <v>0</v>
       </c>
       <c r="AM213" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214" spans="1:39">
@@ -26035,7 +26035,7 @@
         <v>0</v>
       </c>
       <c r="AM223" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224" spans="1:39">
@@ -26195,7 +26195,7 @@
         <v>0</v>
       </c>
       <c r="O225" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P225" t="s">
         <v>0</v>
@@ -26311,7 +26311,7 @@
         <v>0</v>
       </c>
       <c r="O226" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P226" t="s">
         <v>0</v>
@@ -26567,7 +26567,7 @@
         <v>0</v>
       </c>
       <c r="W228" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X228" t="s">
         <v>0</v>
@@ -26606,7 +26606,7 @@
         <v>0</v>
       </c>
       <c r="AJ228" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK228" t="s">
         <v>0</v>
@@ -26781,7 +26781,7 @@
         <v>0</v>
       </c>
       <c r="Q230" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R230" t="s">
         <v>0</v>
@@ -27275,7 +27275,7 @@
         <v>0</v>
       </c>
       <c r="AA234" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB234" t="s">
         <v>0</v>
@@ -28004,7 +28004,7 @@
         <v>0</v>
       </c>
       <c r="AL240" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AM240" t="s">
         <v>0</v>
@@ -28102,7 +28102,7 @@
         <v>1</v>
       </c>
       <c r="AF241" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG241" t="s">
         <v>0</v>
@@ -28625,7 +28625,7 @@
         <v>0</v>
       </c>
       <c r="M246" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N246" t="s">
         <v>0</v>
@@ -28842,7 +28842,7 @@
         <v>0</v>
       </c>
       <c r="H248" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I248" t="s">
         <v>0</v>
@@ -28863,7 +28863,7 @@
         <v>0</v>
       </c>
       <c r="O248" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P248" t="s">
         <v>0</v>
@@ -28976,7 +28976,7 @@
         <v>0</v>
       </c>
       <c r="N249" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O249" t="s">
         <v>1</v>
@@ -29217,7 +29217,7 @@
         <v>0</v>
       </c>
       <c r="Q251" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R251" t="s">
         <v>0</v>
@@ -29244,7 +29244,7 @@
         <v>0</v>
       </c>
       <c r="Z251" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA251" t="s">
         <v>1</v>
@@ -29271,7 +29271,7 @@
         <v>0</v>
       </c>
       <c r="AI251" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ251" t="s">
         <v>0</v>
@@ -29559,7 +29559,7 @@
         <v>0</v>
       </c>
       <c r="O254" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P254" t="s">
         <v>0</v>
@@ -29574,7 +29574,7 @@
         <v>0</v>
       </c>
       <c r="T254" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U254" t="s">
         <v>1</v>
@@ -29598,7 +29598,7 @@
         <v>0</v>
       </c>
       <c r="AB254" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC254" t="s">
         <v>0</v>
@@ -29693,13 +29693,13 @@
         <v>0</v>
       </c>
       <c r="U255" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V255" t="s">
         <v>0</v>
       </c>
       <c r="W255" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X255" t="s">
         <v>0</v>
@@ -29752,7 +29752,7 @@
     </row>
     <row r="256" spans="1:39">
       <c r="B256" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C256" t="s">
         <v>0</v>
@@ -29874,7 +29874,7 @@
         <v>0</v>
       </c>
       <c r="D257" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E257" t="s">
         <v>0</v>
@@ -29889,7 +29889,7 @@
         <v>0</v>
       </c>
       <c r="I257" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J257" t="s">
         <v>0</v>
@@ -29913,7 +29913,7 @@
         <v>0</v>
       </c>
       <c r="Q257" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R257" t="s">
         <v>1</v>
@@ -30175,7 +30175,7 @@
         <v>0</v>
       </c>
       <c r="AA259" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB259" t="s">
         <v>0</v>
@@ -30472,7 +30472,7 @@
         <v>1</v>
       </c>
       <c r="J262" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K262" t="s">
         <v>0</v>
@@ -30669,7 +30669,7 @@
         <v>0</v>
       </c>
       <c r="AK263" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL263" t="s">
         <v>0</v>
@@ -30710,7 +30710,7 @@
         <v>0</v>
       </c>
       <c r="L264" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M264" t="s">
         <v>0</v>
@@ -30814,7 +30814,7 @@
         <v>0</v>
       </c>
       <c r="H265" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I265" t="s">
         <v>1</v>
@@ -30942,7 +30942,7 @@
         <v>1</v>
       </c>
       <c r="L266" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M266" t="s">
         <v>0</v>
@@ -30987,7 +30987,7 @@
         <v>0</v>
       </c>
       <c r="AA266" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB266" t="s">
         <v>0</v>
@@ -31150,7 +31150,7 @@
         <v>1</v>
       </c>
       <c r="D268" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E268" t="s">
         <v>0</v>
@@ -31177,7 +31177,7 @@
         <v>1</v>
       </c>
       <c r="M268" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N268" t="s">
         <v>1</v>
@@ -31564,7 +31564,7 @@
         <v>0</v>
       </c>
       <c r="Z271" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA271" t="s">
         <v>0</v>
@@ -31665,7 +31665,7 @@
         <v>0</v>
       </c>
       <c r="U272" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V272" t="s">
         <v>1</v>
@@ -31995,13 +31995,13 @@
         <v>1</v>
       </c>
       <c r="O275" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P275" t="s">
         <v>0</v>
       </c>
       <c r="Q275" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R275" t="s">
         <v>1</v>
@@ -32099,7 +32099,7 @@
         <v>1</v>
       </c>
       <c r="K276" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L276" t="s">
         <v>0</v>
@@ -32162,7 +32162,7 @@
         <v>0</v>
       </c>
       <c r="AF276" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG276" t="s">
         <v>0</v>
@@ -32183,7 +32183,7 @@
         <v>1</v>
       </c>
       <c r="AM276" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="277" spans="1:39">
@@ -32227,7 +32227,7 @@
         <v>2</v>
       </c>
       <c r="O277" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P277" t="s">
         <v>0</v>
@@ -32370,7 +32370,7 @@
         <v>2</v>
       </c>
       <c r="X278" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y278" t="s">
         <v>0</v>
@@ -32536,7 +32536,7 @@
     </row>
     <row r="280" spans="1:39">
       <c r="B280" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C280" t="s">
         <v>1</v>
@@ -32611,7 +32611,7 @@
         <v>1</v>
       </c>
       <c r="AA280" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB280" t="s">
         <v>0</v>
@@ -32715,7 +32715,7 @@
         <v>0</v>
       </c>
       <c r="W281" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X281" t="s">
         <v>0</v>
@@ -32771,16 +32771,16 @@
         <v>1</v>
       </c>
       <c r="C282" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D282" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E282" t="s">
         <v>0</v>
       </c>
       <c r="F282" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G282" t="s">
         <v>0</v>
@@ -32887,7 +32887,7 @@
         <v>1</v>
       </c>
       <c r="C283" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D283" t="s">
         <v>1</v>
@@ -33200,7 +33200,7 @@
         <v>0</v>
       </c>
       <c r="AD285" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE285" t="s">
         <v>0</v>
@@ -33221,7 +33221,7 @@
         <v>2</v>
       </c>
       <c r="AK285" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL285" t="s">
         <v>1</v>
@@ -33363,7 +33363,7 @@
         <v>1</v>
       </c>
       <c r="G287" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H287" t="s">
         <v>0</v>
@@ -33375,7 +33375,7 @@
         <v>0</v>
       </c>
       <c r="K287" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L287" t="s">
         <v>0</v>
@@ -33390,7 +33390,7 @@
         <v>1</v>
       </c>
       <c r="P287" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q287" t="s">
         <v>2</v>
@@ -33435,7 +33435,7 @@
         <v>0</v>
       </c>
       <c r="AE287" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF287" t="s">
         <v>0</v>
@@ -33473,7 +33473,7 @@
         <v>0</v>
       </c>
       <c r="E288" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F288" t="s">
         <v>0</v>
@@ -33509,7 +33509,7 @@
         <v>1</v>
       </c>
       <c r="Q288" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R288" t="s">
         <v>0</v>
@@ -33518,7 +33518,7 @@
         <v>0</v>
       </c>
       <c r="T288" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U288" t="s">
         <v>2</v>
@@ -33622,7 +33622,7 @@
         <v>0</v>
       </c>
       <c r="P289" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q289" t="s">
         <v>0</v>
@@ -33667,7 +33667,7 @@
         <v>0</v>
       </c>
       <c r="AE289" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF289" t="s">
         <v>0</v>
@@ -33691,7 +33691,7 @@
         <v>0</v>
       </c>
       <c r="AM289" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="290" spans="1:39">
@@ -33705,7 +33705,7 @@
         <v>0</v>
       </c>
       <c r="E290" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F290" t="s">
         <v>0</v>
@@ -33735,10 +33735,10 @@
         <v>0</v>
       </c>
       <c r="O290" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P290" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q290" t="s">
         <v>0</v>
@@ -33786,7 +33786,7 @@
         <v>0</v>
       </c>
       <c r="AF290" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG290" t="s">
         <v>0</v>
@@ -33795,7 +33795,7 @@
         <v>0</v>
       </c>
       <c r="AI290" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ290" t="s">
         <v>0</v>
@@ -33836,7 +33836,7 @@
         <v>1</v>
       </c>
       <c r="J291" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K291" t="s">
         <v>0</v>
@@ -33860,7 +33860,7 @@
         <v>0</v>
       </c>
       <c r="R291" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S291" t="s">
         <v>0</v>
@@ -33875,7 +33875,7 @@
         <v>0</v>
       </c>
       <c r="W291" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X291" t="s">
         <v>0</v>
@@ -33902,7 +33902,7 @@
         <v>0</v>
       </c>
       <c r="AF291" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG291" t="s">
         <v>0</v>
@@ -33911,7 +33911,7 @@
         <v>0</v>
       </c>
       <c r="AI291" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ291" t="s">
         <v>1</v>
@@ -33949,7 +33949,7 @@
         <v>0</v>
       </c>
       <c r="I292" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J292" t="s">
         <v>0</v>
@@ -33961,10 +33961,10 @@
         <v>0</v>
       </c>
       <c r="M292" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N292" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O292" t="s">
         <v>0</v>
@@ -34036,7 +34036,7 @@
         <v>0</v>
       </c>
       <c r="AL292" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM292" t="s">
         <v>0</v>
@@ -34268,7 +34268,7 @@
         <v>0</v>
       </c>
       <c r="AL294" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM294" t="s">
         <v>0</v>
@@ -34288,7 +34288,7 @@
         <v>0</v>
       </c>
       <c r="F295" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G295" t="s">
         <v>1</v>
@@ -34369,7 +34369,7 @@
         <v>0</v>
       </c>
       <c r="AG295" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH295" t="s">
         <v>1</v>
@@ -34464,7 +34464,7 @@
         <v>0</v>
       </c>
       <c r="Z296" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA296" t="s">
         <v>0</v>
@@ -34550,7 +34550,7 @@
         <v>0</v>
       </c>
       <c r="P297" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q297" t="s">
         <v>2</v>
@@ -34639,7 +34639,7 @@
         <v>0</v>
       </c>
       <c r="G298" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H298" t="s">
         <v>1</v>
@@ -34699,13 +34699,13 @@
         <v>1</v>
       </c>
       <c r="AA298" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB298" t="s">
         <v>2</v>
       </c>
       <c r="AC298" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD298" t="s">
         <v>2</v>
@@ -34726,7 +34726,7 @@
         <v>0</v>
       </c>
       <c r="AJ298" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK298" t="s">
         <v>0</v>
@@ -34794,7 +34794,7 @@
         <v>0</v>
       </c>
       <c r="T299" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U299" t="s">
         <v>1</v>
@@ -34886,7 +34886,7 @@
         <v>0</v>
       </c>
       <c r="L300" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M300" t="s">
         <v>0</v>
@@ -34931,7 +34931,7 @@
         <v>0</v>
       </c>
       <c r="AA300" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB300" t="s">
         <v>1</v>
@@ -34946,7 +34946,7 @@
         <v>0</v>
       </c>
       <c r="AF300" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG300" t="s">
         <v>0</v>
@@ -35002,7 +35002,7 @@
         <v>1</v>
       </c>
       <c r="L301" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M301" t="s">
         <v>1</v>
@@ -35175,7 +35175,7 @@
         <v>0</v>
       </c>
       <c r="AE302" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF302" t="s">
         <v>2</v>
@@ -35264,7 +35264,7 @@
         <v>1</v>
       </c>
       <c r="V303" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W303" t="s">
         <v>0</v>
@@ -35279,7 +35279,7 @@
         <v>0</v>
       </c>
       <c r="AA303" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB303" t="s">
         <v>0</v>
@@ -35303,7 +35303,7 @@
         <v>0</v>
       </c>
       <c r="AI303" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ303" t="s">
         <v>1</v>
@@ -35338,7 +35338,7 @@
         <v>0</v>
       </c>
       <c r="H304" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I304" t="s">
         <v>1</v>
@@ -35356,7 +35356,7 @@
         <v>0</v>
       </c>
       <c r="N304" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O304" t="s">
         <v>1</v>
@@ -35422,7 +35422,7 @@
         <v>2</v>
       </c>
       <c r="AJ304" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK304" t="s">
         <v>0</v>
@@ -35532,7 +35532,7 @@
         <v>0</v>
       </c>
       <c r="AH305" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI305" t="s">
         <v>1</v>
@@ -35677,7 +35677,7 @@
         <v>0</v>
       </c>
       <c r="E307" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F307" t="s">
         <v>1</v>
@@ -35686,7 +35686,7 @@
         <v>1</v>
       </c>
       <c r="H307" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I307" t="s">
         <v>0</v>
@@ -35704,7 +35704,7 @@
         <v>0</v>
       </c>
       <c r="N307" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O307" t="s">
         <v>1</v>
@@ -35716,7 +35716,7 @@
         <v>2</v>
       </c>
       <c r="R307" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S307" t="s">
         <v>1</v>
@@ -35761,13 +35761,13 @@
         <v>0</v>
       </c>
       <c r="AG307" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH307" t="s">
         <v>0</v>
       </c>
       <c r="AI307" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ307" t="s">
         <v>2</v>
@@ -35776,7 +35776,7 @@
         <v>0</v>
       </c>
       <c r="AL307" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM307" t="s">
         <v>0</v>
@@ -35871,7 +35871,7 @@
         <v>0</v>
       </c>
       <c r="AE308" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF308" t="s">
         <v>0</v>
@@ -35886,13 +35886,13 @@
         <v>1</v>
       </c>
       <c r="AJ308" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK308" t="s">
         <v>0</v>
       </c>
       <c r="AL308" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM308" t="s">
         <v>1</v>
@@ -35903,7 +35903,7 @@
         <v>0</v>
       </c>
       <c r="C309" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D309" t="s">
         <v>0</v>
@@ -35951,7 +35951,7 @@
         <v>0</v>
       </c>
       <c r="S309" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T309" t="s">
         <v>0</v>
@@ -35987,7 +35987,7 @@
         <v>0</v>
       </c>
       <c r="AE309" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF309" t="s">
         <v>0</v>
@@ -36008,10 +36008,10 @@
         <v>0</v>
       </c>
       <c r="AL309" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM309" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="310" spans="1:39">
@@ -36019,7 +36019,7 @@
         <v>0</v>
       </c>
       <c r="C310" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D310" t="s">
         <v>0</v>
@@ -36076,7 +36076,7 @@
         <v>1</v>
       </c>
       <c r="V310" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W310" t="s">
         <v>1</v>
@@ -36124,7 +36124,7 @@
         <v>0</v>
       </c>
       <c r="AL310" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM310" t="s">
         <v>1</v>
@@ -36138,7 +36138,7 @@
         <v>1</v>
       </c>
       <c r="D311" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E311" t="s">
         <v>1</v>
@@ -36162,7 +36162,7 @@
         <v>1</v>
       </c>
       <c r="L311" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M311" t="s">
         <v>1</v>
@@ -36177,7 +36177,7 @@
         <v>1</v>
       </c>
       <c r="Q311" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R311" t="s">
         <v>0</v>
@@ -36204,7 +36204,7 @@
         <v>1</v>
       </c>
       <c r="Z311" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA311" t="s">
         <v>2</v>
@@ -36290,7 +36290,7 @@
         <v>0</v>
       </c>
       <c r="P312" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q312" t="s">
         <v>0</v>
@@ -36311,7 +36311,7 @@
         <v>0</v>
       </c>
       <c r="W312" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X312" t="s">
         <v>0</v>
@@ -36367,7 +36367,7 @@
         <v>0</v>
       </c>
       <c r="C313" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D313" t="s">
         <v>1</v>
@@ -36394,7 +36394,7 @@
         <v>0</v>
       </c>
       <c r="L313" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M313" t="s">
         <v>0</v>
@@ -36427,7 +36427,7 @@
         <v>0</v>
       </c>
       <c r="W313" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X313" t="s">
         <v>0</v>
@@ -36668,37 +36668,37 @@
         <v>0</v>
       </c>
       <c r="Z315" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA315" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB315" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC315" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD315" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE315" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF315" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG315" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH315" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI315" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ315" t="s">
         <v>3</v>
-      </c>
-      <c r="AA315" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB315" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC315" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD315" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE315" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF315" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG315" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH315" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI315" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ315" t="s">
-        <v>1</v>
       </c>
       <c r="AK315" t="s">
         <v>2</v>
@@ -36712,7 +36712,7 @@
     </row>
     <row r="316" spans="1:39">
       <c r="B316" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C316" t="s">
         <v>0</v>
@@ -36763,7 +36763,7 @@
         <v>0</v>
       </c>
       <c r="S316" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T316" t="s">
         <v>1</v>
@@ -36787,7 +36787,7 @@
         <v>0</v>
       </c>
       <c r="AA316" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB316" t="s">
         <v>2</v>
@@ -36814,16 +36814,16 @@
         <v>0</v>
       </c>
       <c r="AJ316" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK316" t="s">
         <v>1</v>
       </c>
       <c r="AL316" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM316" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:39">
@@ -36873,13 +36873,13 @@
         <v>0</v>
       </c>
       <c r="Q317" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R317" t="s">
         <v>1</v>
       </c>
       <c r="S317" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T317" t="s">
         <v>0</v>
@@ -36906,7 +36906,7 @@
         <v>2</v>
       </c>
       <c r="AB317" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC317" t="s">
         <v>1</v>
@@ -36915,13 +36915,13 @@
         <v>0</v>
       </c>
       <c r="AE317" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF317" t="s">
         <v>0</v>
       </c>
       <c r="AG317" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH317" t="s">
         <v>0</v>
@@ -36953,7 +36953,7 @@
         <v>0</v>
       </c>
       <c r="E318" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F318" t="s">
         <v>0</v>
@@ -36983,7 +36983,7 @@
         <v>1</v>
       </c>
       <c r="O318" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P318" t="s">
         <v>3</v>
@@ -37007,7 +37007,7 @@
         <v>1</v>
       </c>
       <c r="W318" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X318" t="s">
         <v>0</v>
@@ -37093,7 +37093,7 @@
         <v>1</v>
       </c>
       <c r="M319" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N319" t="s">
         <v>0</v>
@@ -37162,13 +37162,13 @@
         <v>0</v>
       </c>
       <c r="AJ319" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK319" t="s">
         <v>0</v>
       </c>
       <c r="AL319" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM319" t="s">
         <v>1</v>
@@ -37227,7 +37227,7 @@
         <v>1</v>
       </c>
       <c r="S320" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T320" t="s">
         <v>2</v>
@@ -37281,7 +37281,7 @@
         <v>2</v>
       </c>
       <c r="AK320" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL320" t="s">
         <v>2</v>
@@ -37316,7 +37316,7 @@
         <v>1</v>
       </c>
       <c r="J321" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K321" t="s">
         <v>2</v>
@@ -37423,7 +37423,7 @@
         <v>0</v>
       </c>
       <c r="G322" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H322" t="s">
         <v>1</v>
@@ -37447,7 +37447,7 @@
         <v>0</v>
       </c>
       <c r="O322" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P322" t="s">
         <v>1</v>
@@ -37495,7 +37495,7 @@
         <v>1</v>
       </c>
       <c r="AE322" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF322" t="s">
         <v>1</v>
@@ -37524,7 +37524,7 @@
     </row>
     <row r="323" spans="1:39">
       <c r="B323" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C323" t="s">
         <v>1</v>
@@ -37587,7 +37587,7 @@
         <v>2</v>
       </c>
       <c r="W323" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X323" t="s">
         <v>0</v>
@@ -37617,7 +37617,7 @@
         <v>0</v>
       </c>
       <c r="AG323" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH323" t="s">
         <v>0</v>
@@ -37703,7 +37703,7 @@
         <v>2</v>
       </c>
       <c r="W324" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X324" t="s">
         <v>0</v>
@@ -37739,7 +37739,7 @@
         <v>0</v>
       </c>
       <c r="AI324" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ324" t="s">
         <v>1</v>
@@ -37819,7 +37819,7 @@
         <v>0</v>
       </c>
       <c r="W325" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X325" t="s">
         <v>0</v>
@@ -37890,7 +37890,7 @@
         <v>1</v>
       </c>
       <c r="H326" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I326" t="s">
         <v>2</v>
@@ -37953,7 +37953,7 @@
         <v>0</v>
       </c>
       <c r="AC326" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD326" t="s">
         <v>0</v>
@@ -37983,7 +37983,7 @@
         <v>0</v>
       </c>
       <c r="AM326" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="327" spans="1:39">
@@ -38018,7 +38018,7 @@
         <v>1</v>
       </c>
       <c r="L327" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M327" t="s">
         <v>0</v>
@@ -38045,7 +38045,7 @@
         <v>0</v>
       </c>
       <c r="U327" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V327" t="s">
         <v>0</v>
@@ -38084,7 +38084,7 @@
         <v>1</v>
       </c>
       <c r="AH327" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AI327" t="s">
         <v>1</v>
@@ -38107,7 +38107,7 @@
         <v>1</v>
       </c>
       <c r="C328" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D328" t="s">
         <v>0</v>
@@ -38137,7 +38137,7 @@
         <v>2</v>
       </c>
       <c r="M328" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N328" t="s">
         <v>1</v>
@@ -38167,7 +38167,7 @@
         <v>0</v>
       </c>
       <c r="W328" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X328" t="s">
         <v>2</v>
@@ -38220,7 +38220,7 @@
     </row>
     <row r="329" spans="1:39">
       <c r="B329" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C329" t="s">
         <v>1</v>
@@ -38339,7 +38339,7 @@
         <v>2</v>
       </c>
       <c r="C330" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D330" t="s">
         <v>1</v>
@@ -38351,7 +38351,7 @@
         <v>0</v>
       </c>
       <c r="G330" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H330" t="s">
         <v>2</v>
@@ -38378,7 +38378,7 @@
         <v>0</v>
       </c>
       <c r="P330" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q330" t="s">
         <v>3</v>
@@ -38414,7 +38414,7 @@
         <v>0</v>
       </c>
       <c r="AB330" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC330" t="s">
         <v>1</v>
@@ -38426,7 +38426,7 @@
         <v>0</v>
       </c>
       <c r="AF330" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG330" t="s">
         <v>0</v>
@@ -38488,7 +38488,7 @@
         <v>0</v>
       </c>
       <c r="N331" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O331" t="s">
         <v>0</v>
@@ -38699,13 +38699,13 @@
         <v>0</v>
       </c>
       <c r="G333" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H333" t="s">
         <v>0</v>
       </c>
       <c r="I333" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J333" t="s">
         <v>1</v>
@@ -38753,10 +38753,10 @@
         <v>0</v>
       </c>
       <c r="Y333" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z333" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA333" t="s">
         <v>0</v>
@@ -38777,7 +38777,7 @@
         <v>2</v>
       </c>
       <c r="AG333" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH333" t="s">
         <v>1</v>
@@ -38824,13 +38824,13 @@
         <v>2</v>
       </c>
       <c r="J334" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K334" t="s">
         <v>0</v>
       </c>
       <c r="L334" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M334" t="s">
         <v>1</v>
@@ -38881,7 +38881,7 @@
         <v>2</v>
       </c>
       <c r="AC334" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD334" t="s">
         <v>1</v>
@@ -38902,7 +38902,7 @@
         <v>2</v>
       </c>
       <c r="AJ334" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK334" t="s">
         <v>0</v>
@@ -38955,7 +38955,7 @@
         <v>0</v>
       </c>
       <c r="O335" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P335" t="s">
         <v>0</v>
@@ -38976,7 +38976,7 @@
         <v>0</v>
       </c>
       <c r="V335" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W335" t="s">
         <v>0</v>
@@ -38988,13 +38988,13 @@
         <v>3</v>
       </c>
       <c r="Z335" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA335" t="s">
         <v>1</v>
       </c>
       <c r="AB335" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC335" t="s">
         <v>1</v>
@@ -39059,7 +39059,7 @@
         <v>2</v>
       </c>
       <c r="K336" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L336" t="s">
         <v>0</v>
@@ -39080,7 +39080,7 @@
         <v>0</v>
       </c>
       <c r="R336" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S336" t="s">
         <v>2</v>
@@ -39157,7 +39157,7 @@
         <v>1</v>
       </c>
       <c r="E337" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F337" t="s">
         <v>0</v>
@@ -39172,7 +39172,7 @@
         <v>3</v>
       </c>
       <c r="J337" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K337" t="s">
         <v>0</v>
@@ -39196,7 +39196,7 @@
         <v>0</v>
       </c>
       <c r="R337" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S337" t="s">
         <v>0</v>
@@ -39205,7 +39205,7 @@
         <v>0</v>
       </c>
       <c r="U337" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V337" t="s">
         <v>0</v>
@@ -39244,7 +39244,7 @@
         <v>2</v>
       </c>
       <c r="AH337" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI337" t="s">
         <v>0</v>
@@ -39264,7 +39264,7 @@
     </row>
     <row r="338" spans="1:39">
       <c r="B338" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C338" t="s">
         <v>1</v>
@@ -39285,16 +39285,16 @@
         <v>0</v>
       </c>
       <c r="I338" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J338" t="s">
         <v>1</v>
       </c>
       <c r="K338" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L338" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M338" t="s">
         <v>3</v>
@@ -39312,7 +39312,7 @@
         <v>0</v>
       </c>
       <c r="R338" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S338" t="s">
         <v>1</v>
@@ -39333,7 +39333,7 @@
         <v>0</v>
       </c>
       <c r="Y338" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z338" t="s">
         <v>1</v>
@@ -39410,7 +39410,7 @@
         <v>2</v>
       </c>
       <c r="L339" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M339" t="s">
         <v>0</v>
@@ -39565,7 +39565,7 @@
         <v>0</v>
       </c>
       <c r="Y340" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z340" t="s">
         <v>1</v>
@@ -39618,7 +39618,7 @@
         <v>0</v>
       </c>
       <c r="D341" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E341" t="s">
         <v>0</v>
@@ -39675,7 +39675,7 @@
         <v>2</v>
       </c>
       <c r="W341" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X341" t="s">
         <v>0</v>
@@ -39705,7 +39705,7 @@
         <v>0</v>
       </c>
       <c r="AG341" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH341" t="s">
         <v>1</v>
@@ -39785,32 +39785,32 @@
         <v>3</v>
       </c>
       <c r="U342" t="s">
+        <v>2</v>
+      </c>
+      <c r="V342" t="s">
+        <v>1</v>
+      </c>
+      <c r="W342" t="s">
+        <v>2</v>
+      </c>
+      <c r="X342" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y342" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z342" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA342" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB342" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC342" t="s">
         <v>3</v>
       </c>
-      <c r="V342" t="s">
-        <v>1</v>
-      </c>
-      <c r="W342" t="s">
-        <v>2</v>
-      </c>
-      <c r="X342" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y342" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z342" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA342" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB342" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC342" t="s">
-        <v>0</v>
-      </c>
       <c r="AD342" t="s">
         <v>0</v>
       </c>
@@ -39839,7 +39839,7 @@
         <v>0</v>
       </c>
       <c r="AM342" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="343" spans="1:39">
@@ -39919,7 +39919,7 @@
         <v>0</v>
       </c>
       <c r="AA343" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB343" t="s">
         <v>1</v>
@@ -39978,7 +39978,7 @@
         <v>1</v>
       </c>
       <c r="H344" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I344" t="s">
         <v>0</v>
@@ -39993,7 +39993,7 @@
         <v>0</v>
       </c>
       <c r="M344" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N344" t="s">
         <v>0</v>
@@ -40154,7 +40154,7 @@
         <v>0</v>
       </c>
       <c r="AB345" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC345" t="s">
         <v>2</v>
@@ -40178,13 +40178,13 @@
         <v>1</v>
       </c>
       <c r="AJ345" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK345" t="s">
         <v>0</v>
       </c>
       <c r="AL345" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM345" t="s">
         <v>1</v>
@@ -40323,7 +40323,7 @@
         <v>0</v>
       </c>
       <c r="G347" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H347" t="s">
         <v>1</v>
@@ -40484,7 +40484,7 @@
         <v>1</v>
       </c>
       <c r="V348" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W348" t="s">
         <v>0</v>
@@ -40511,7 +40511,7 @@
         <v>1</v>
       </c>
       <c r="AE348" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF348" t="s">
         <v>0</v>
@@ -40523,7 +40523,7 @@
         <v>1</v>
       </c>
       <c r="AI348" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ348" t="s">
         <v>0</v>
@@ -40665,28 +40665,28 @@
         <v>0</v>
       </c>
       <c r="E350" t="s">
+        <v>2</v>
+      </c>
+      <c r="F350" t="s">
+        <v>1</v>
+      </c>
+      <c r="G350" t="s">
+        <v>0</v>
+      </c>
+      <c r="H350" t="s">
+        <v>1</v>
+      </c>
+      <c r="I350" t="s">
+        <v>1</v>
+      </c>
+      <c r="J350" t="s">
+        <v>1</v>
+      </c>
+      <c r="K350" t="s">
+        <v>1</v>
+      </c>
+      <c r="L350" t="s">
         <v>3</v>
-      </c>
-      <c r="F350" t="s">
-        <v>1</v>
-      </c>
-      <c r="G350" t="s">
-        <v>0</v>
-      </c>
-      <c r="H350" t="s">
-        <v>0</v>
-      </c>
-      <c r="I350" t="s">
-        <v>1</v>
-      </c>
-      <c r="J350" t="s">
-        <v>1</v>
-      </c>
-      <c r="K350" t="s">
-        <v>1</v>
-      </c>
-      <c r="L350" t="s">
-        <v>0</v>
       </c>
       <c r="M350" t="s">
         <v>0</v>
@@ -40847,7 +40847,7 @@
         <v>0</v>
       </c>
       <c r="AA351" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AB351" t="s">
         <v>0</v>
@@ -40963,7 +40963,7 @@
         <v>0</v>
       </c>
       <c r="AA352" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB352" t="s">
         <v>0</v>
@@ -40993,7 +40993,7 @@
         <v>1</v>
       </c>
       <c r="AK352" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL352" t="s">
         <v>3</v>
@@ -41150,7 +41150,7 @@
         <v>0</v>
       </c>
       <c r="L354" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M354" t="s">
         <v>1</v>
@@ -41162,7 +41162,7 @@
         <v>1</v>
       </c>
       <c r="P354" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q354" t="s">
         <v>0</v>
@@ -41174,13 +41174,13 @@
         <v>2</v>
       </c>
       <c r="T354" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U354" t="s">
         <v>0</v>
       </c>
       <c r="V354" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W354" t="s">
         <v>1</v>
@@ -41266,7 +41266,7 @@
         <v>0</v>
       </c>
       <c r="L355" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M355" t="s">
         <v>2</v>
@@ -41275,7 +41275,7 @@
         <v>1</v>
       </c>
       <c r="O355" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P355" t="s">
         <v>1</v>
@@ -41394,7 +41394,7 @@
         <v>1</v>
       </c>
       <c r="P356" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q356" t="s">
         <v>0</v>
@@ -41424,7 +41424,7 @@
         <v>0</v>
       </c>
       <c r="Z356" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA356" t="s">
         <v>0</v>
@@ -41433,7 +41433,7 @@
         <v>0</v>
       </c>
       <c r="AC356" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD356" t="s">
         <v>2</v>
@@ -41495,7 +41495,7 @@
         <v>0</v>
       </c>
       <c r="K357" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L357" t="s">
         <v>1</v>
@@ -41561,10 +41561,10 @@
         <v>0</v>
       </c>
       <c r="AG357" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH357" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI357" t="s">
         <v>0</v>
@@ -41709,7 +41709,7 @@
         <v>1</v>
       </c>
       <c r="E359" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F359" t="s">
         <v>3</v>
@@ -41742,10 +41742,10 @@
         <v>0</v>
       </c>
       <c r="P359" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q359" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R359" t="s">
         <v>3</v>
@@ -41772,7 +41772,7 @@
         <v>1</v>
       </c>
       <c r="Z359" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA359" t="s">
         <v>1</v>
@@ -41781,7 +41781,7 @@
         <v>0</v>
       </c>
       <c r="AC359" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD359" t="s">
         <v>1</v>
@@ -41808,7 +41808,7 @@
         <v>0</v>
       </c>
       <c r="AL359" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AM359" t="s">
         <v>1</v>
@@ -41837,7 +41837,7 @@
         <v>0</v>
       </c>
       <c r="I360" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J360" t="s">
         <v>0</v>
@@ -41935,7 +41935,7 @@
         <v>0</v>
       </c>
       <c r="C361" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D361" t="s">
         <v>0</v>
@@ -41944,13 +41944,13 @@
         <v>2</v>
       </c>
       <c r="F361" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G361" t="s">
         <v>1</v>
       </c>
       <c r="H361" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I361" t="s">
         <v>0</v>
@@ -42037,7 +42037,7 @@
         <v>0</v>
       </c>
       <c r="AK361" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL361" t="s">
         <v>0</v>
@@ -42051,7 +42051,7 @@
         <v>0</v>
       </c>
       <c r="C362" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D362" t="s">
         <v>0</v>
@@ -42072,7 +42072,7 @@
         <v>0</v>
       </c>
       <c r="J362" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K362" t="s">
         <v>0</v>
@@ -42188,7 +42188,7 @@
         <v>0</v>
       </c>
       <c r="J363" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K363" t="s">
         <v>0</v>
@@ -42289,7 +42289,7 @@
         <v>0</v>
       </c>
       <c r="E364" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F364" t="s">
         <v>0</v>
@@ -42313,7 +42313,7 @@
         <v>0</v>
       </c>
       <c r="M364" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N364" t="s">
         <v>0</v>
@@ -42343,13 +42343,13 @@
         <v>0</v>
       </c>
       <c r="W364" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X364" t="s">
         <v>0</v>
       </c>
       <c r="Y364" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z364" t="s">
         <v>0</v>
@@ -42391,7 +42391,7 @@
         <v>2</v>
       </c>
       <c r="AM364" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="365" spans="1:39">
@@ -42495,7 +42495,7 @@
         <v>1</v>
       </c>
       <c r="AI365" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ365" t="s">
         <v>1</v>
@@ -42527,10 +42527,10 @@
         <v>1</v>
       </c>
       <c r="G366" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H366" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I366" t="s">
         <v>0</v>
@@ -42563,7 +42563,7 @@
         <v>1</v>
       </c>
       <c r="S366" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T366" t="s">
         <v>0</v>
@@ -42730,7 +42730,7 @@
         <v>1</v>
       </c>
       <c r="AJ367" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK367" t="s">
         <v>0</v>

</xml_diff>